<commit_message>
adjust class name, add test case (runs out of heap space)
</commit_message>
<xml_diff>
--- a/bin/main/PipelineTimings.xlsx
+++ b/bin/main/PipelineTimings.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Code\GradleImageTransformationProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F735CA0-DCAD-4274-A6CD-9B000F19376E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EE4559-BD4F-47E8-B144-1C6FB05D5EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="from a jar file all equal" sheetId="3" r:id="rId1"/>
-    <sheet name="all equal in comp background" sheetId="2" r:id="rId2"/>
+    <sheet name="VS Code all equal" sheetId="2" r:id="rId2"/>
     <sheet name="random results" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -221,34 +221,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27340</c:v>
+                  <c:v>26019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16290</c:v>
+                  <c:v>20708</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14471</c:v>
+                  <c:v>15666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12831</c:v>
+                  <c:v>14784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12286</c:v>
+                  <c:v>12139</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12727</c:v>
+                  <c:v>12123</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13102</c:v>
+                  <c:v>12197</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12514</c:v>
+                  <c:v>11781</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12125</c:v>
+                  <c:v>11956</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12857</c:v>
+                  <c:v>11957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -305,34 +305,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14441</c:v>
+                  <c:v>17203</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10722</c:v>
+                  <c:v>13457</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11162</c:v>
+                  <c:v>12744</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11636</c:v>
+                  <c:v>12600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11246</c:v>
+                  <c:v>12927</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11091</c:v>
+                  <c:v>12748</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10876</c:v>
+                  <c:v>13883</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11148</c:v>
+                  <c:v>12852</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11267</c:v>
+                  <c:v>12936</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11375</c:v>
+                  <c:v>13645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,34 +389,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14147</c:v>
+                  <c:v>16343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11214</c:v>
+                  <c:v>13463</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11635</c:v>
+                  <c:v>13958</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11805</c:v>
+                  <c:v>14375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11907</c:v>
+                  <c:v>14130</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11961</c:v>
+                  <c:v>14241</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11813</c:v>
+                  <c:v>14139</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11854</c:v>
+                  <c:v>13819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12126</c:v>
+                  <c:v>13547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11839</c:v>
+                  <c:v>13905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -473,34 +473,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>13618</c:v>
+                  <c:v>17303</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10888</c:v>
+                  <c:v>13200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11523</c:v>
+                  <c:v>13170</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11655</c:v>
+                  <c:v>13490</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11775</c:v>
+                  <c:v>13479</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12061</c:v>
+                  <c:v>13689</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12229</c:v>
+                  <c:v>12391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11927</c:v>
+                  <c:v>14070</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12205</c:v>
+                  <c:v>13862</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12125</c:v>
+                  <c:v>13833</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,7 +914,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'all equal in comp background'!$B$1</c:f>
+              <c:f>'VS Code all equal'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -949,7 +949,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'all equal in comp background'!$B$2:$B$11</c:f>
+              <c:f>'VS Code all equal'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -998,7 +998,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'all equal in comp background'!$C$1</c:f>
+              <c:f>'VS Code all equal'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1033,7 +1033,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'all equal in comp background'!$C$2:$C$11</c:f>
+              <c:f>'VS Code all equal'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1082,7 +1082,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'all equal in comp background'!$D$1</c:f>
+              <c:f>'VS Code all equal'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1117,7 +1117,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'all equal in comp background'!$D$2:$D$11</c:f>
+              <c:f>'VS Code all equal'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1166,7 +1166,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'all equal in comp background'!$E$1</c:f>
+              <c:f>'VS Code all equal'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1201,7 +1201,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'all equal in comp background'!$E$2:$E$11</c:f>
+              <c:f>'VS Code all equal'!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4316,8 +4316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01726E12-08F3-41E8-9B3F-2C1847D63122}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4350,16 +4350,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>27340</v>
+        <v>26019</v>
       </c>
       <c r="C2">
-        <v>14441</v>
+        <v>17203</v>
       </c>
       <c r="D2">
-        <v>14147</v>
+        <v>16343</v>
       </c>
       <c r="E2">
-        <v>13618</v>
+        <v>17303</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4367,16 +4367,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>16290</v>
+        <v>20708</v>
       </c>
       <c r="C3">
-        <v>10722</v>
+        <v>13457</v>
       </c>
       <c r="D3">
-        <v>11214</v>
+        <v>13463</v>
       </c>
       <c r="E3">
-        <v>10888</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4384,16 +4384,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>14471</v>
+        <v>15666</v>
       </c>
       <c r="C4">
-        <v>11162</v>
+        <v>12744</v>
       </c>
       <c r="D4">
-        <v>11635</v>
+        <v>13958</v>
       </c>
       <c r="E4">
-        <v>11523</v>
+        <v>13170</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4401,16 +4401,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>12831</v>
+        <v>14784</v>
       </c>
       <c r="C5">
-        <v>11636</v>
+        <v>12600</v>
       </c>
       <c r="D5">
-        <v>11805</v>
+        <v>14375</v>
       </c>
       <c r="E5">
-        <v>11655</v>
+        <v>13490</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4418,16 +4418,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>12286</v>
+        <v>12139</v>
       </c>
       <c r="C6">
-        <v>11246</v>
+        <v>12927</v>
       </c>
       <c r="D6">
-        <v>11907</v>
+        <v>14130</v>
       </c>
       <c r="E6">
-        <v>11775</v>
+        <v>13479</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4435,16 +4435,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>12727</v>
+        <v>12123</v>
       </c>
       <c r="C7">
-        <v>11091</v>
+        <v>12748</v>
       </c>
       <c r="D7">
-        <v>11961</v>
+        <v>14241</v>
       </c>
       <c r="E7">
-        <v>12061</v>
+        <v>13689</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,16 +4452,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>13102</v>
+        <v>12197</v>
       </c>
       <c r="C8">
-        <v>10876</v>
+        <v>13883</v>
       </c>
       <c r="D8">
-        <v>11813</v>
+        <v>14139</v>
       </c>
       <c r="E8">
-        <v>12229</v>
+        <v>12391</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4469,16 +4469,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>12514</v>
+        <v>11781</v>
       </c>
       <c r="C9">
-        <v>11148</v>
+        <v>12852</v>
       </c>
       <c r="D9">
-        <v>11854</v>
+        <v>13819</v>
       </c>
       <c r="E9">
-        <v>11927</v>
+        <v>14070</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,16 +4486,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>12125</v>
+        <v>11956</v>
       </c>
       <c r="C10">
-        <v>11267</v>
+        <v>12936</v>
       </c>
       <c r="D10">
-        <v>12126</v>
+        <v>13547</v>
       </c>
       <c r="E10">
-        <v>12205</v>
+        <v>13862</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,16 +4503,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>12857</v>
+        <v>11957</v>
       </c>
       <c r="C11">
-        <v>11375</v>
+        <v>13645</v>
       </c>
       <c r="D11">
-        <v>11839</v>
+        <v>13905</v>
       </c>
       <c r="E11">
-        <v>12125</v>
+        <v>13833</v>
       </c>
     </row>
   </sheetData>
@@ -4525,8 +4525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CBAC9B1-47E2-460A-A64F-F2B8B66E2018}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>